<commit_message>
few extra things added, jenkins notes pending
</commit_message>
<xml_diff>
--- a/SelJavaAppium.xlsx
+++ b/SelJavaAppium.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="678" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Selenium" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Jenkins" sheetId="10" r:id="rId10"/>
     <sheet name="Mobile app testing" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="190">
   <si>
     <t>Difference between RC and Webdriver</t>
   </si>
@@ -65,24 +65,12 @@
     <t>how to connect to DB by using selenium</t>
   </si>
   <si>
-    <t>Diff b/w Junit/TestNG</t>
-  </si>
-  <si>
-    <t>Annotations in TestNG</t>
-  </si>
-  <si>
     <t>Reporting in selenium</t>
   </si>
   <si>
     <t>Quit and close</t>
   </si>
   <si>
-    <t>Framework designing</t>
-  </si>
-  <si>
-    <t>use of data provider</t>
-  </si>
-  <si>
     <t>Programmes</t>
   </si>
   <si>
@@ -96,9 +84,6 @@
   </si>
   <si>
     <t>In webpage how do u know a check box,radio button is present</t>
-  </si>
-  <si>
-    <t>excel reading and writing and printing</t>
   </si>
   <si>
     <t>Difference b/w findElement and findElements</t>
@@ -272,9 +257,6 @@
     <t>Finds 1st element in current web,Finds all web elements in webpage</t>
   </si>
   <si>
-    <t>implicit,explicit,fluent</t>
-  </si>
-  <si>
     <t>Robot class</t>
   </si>
   <si>
@@ -308,27 +290,6 @@
   </si>
   <si>
     <t>Installation and execution details</t>
-  </si>
-  <si>
-    <t>TestNG parameters</t>
-  </si>
-  <si>
-    <t>Priority = 1,0</t>
-  </si>
-  <si>
-    <t>enabled = true,false</t>
-  </si>
-  <si>
-    <t>dependsonmethod</t>
-  </si>
-  <si>
-    <t>Parameterized test</t>
-  </si>
-  <si>
-    <t>Passing parameters using dataproviders</t>
-  </si>
-  <si>
-    <t>Passing parameters using testNG.xml - http://www.tutorialspoint.com/testng/testng_parameterized_test.htm</t>
   </si>
   <si>
     <t>By changing number of arguments
@@ -636,12 +597,307 @@
   <si>
     <t>Assert command to check whether the test case passed or failed</t>
   </si>
+  <si>
+    <t>UTIL packages</t>
+  </si>
+  <si>
+    <t>Excel Reader program</t>
+  </si>
+  <si>
+    <t>KeyWord Driven - class file containing static keywords</t>
+  </si>
+  <si>
+    <t>Test Util File - Program which reads data from excel and executes the test case if keyword = "Y"</t>
+  </si>
+  <si>
+    <t>Page Objects - each webelement is treated as separate method and called in test case package</t>
+  </si>
+  <si>
+    <t>PageObjectMethod_Navigation</t>
+  </si>
+  <si>
+    <t>PageObjectMethod_ChangePassword</t>
+  </si>
+  <si>
+    <t>PageObjectMethod_IntripCHange</t>
+  </si>
+  <si>
+    <t>PageObjectMethod_TripFlow</t>
+  </si>
+  <si>
+    <t>Libraries</t>
+  </si>
+  <si>
+    <t>Maven dependencies</t>
+  </si>
+  <si>
+    <t>APK folder</t>
+  </si>
+  <si>
+    <t>TestNG O/P</t>
+  </si>
+  <si>
+    <t>TestNG Groups &amp; depends</t>
+  </si>
+  <si>
+    <t>at Test(groups = {"car"})</t>
+  </si>
+  <si>
+    <t>at Test(dependsOnMethods = {"openBrowser"})</t>
+  </si>
+  <si>
+    <t>TestNG prioritizing &amp; sequencing</t>
+  </si>
+  <si>
+    <t>at Test(priority = 1)</t>
+  </si>
+  <si>
+    <t>at Test(priority = 1 , enabled = false)</t>
+  </si>
+  <si>
+    <t>TestNG reporters and assert</t>
+  </si>
+  <si>
+    <t>TestNG Parameter &amp; dataprovider</t>
+  </si>
+  <si>
+    <t>TestNG listners</t>
+  </si>
+  <si>
+    <t>Benefits</t>
+  </si>
+  <si>
+    <t>Benefits of TestNG</t>
+  </si>
+  <si>
+    <t>There are number of benefits but from Selenium perspective, major advantages of TestNG are :</t>
+  </si>
+  <si>
+    <r>
+      <t>1. It gives the ability to produce </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>HTML Reports</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> of execution</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2. Annotations</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>made testers life easy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3. Test cases can be </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Grouped &amp; Prioritized</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> more easily</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4. Parallel</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>testing is possible</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5. Generates </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Logs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6. Data </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Parameterization</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF38393A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>is possible</t>
+    </r>
+  </si>
+  <si>
+    <t>In selenium there are two types of logging. High level logging and Low level logging. In low level logging you try to produce logs for the every step you take or every action you make in your automation script. In high  level logging you just try to capture main events of your test.</t>
+  </si>
+  <si>
+    <t>Log4J logging - log.info</t>
+  </si>
+  <si>
+    <t>TestNG logging - report.console</t>
+  </si>
+  <si>
+    <t>Assert command stops execution when it fails</t>
+  </si>
+  <si>
+    <t>Assert.assertTrue(),Assert.assertFalse()</t>
+  </si>
+  <si>
+    <t>Assert.assertEquals()</t>
+  </si>
+  <si>
+    <t>at Parameters({"sUsername" , "sPassword"}) - parameters would be passed values in testng.xml</t>
+  </si>
+  <si>
+    <t>&lt;paramter name = "sUsername" value = "test1"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;paramter name = "sUsername" value = "test2"/&gt;</t>
+  </si>
+  <si>
+    <t>Parameterization - reading user name and pass and storing in any test case program. Apache POI API</t>
+  </si>
+  <si>
+    <t>atDataProvider(name = "Authentication")
+  public static Object[][] credentials() {
+        return new Object[][] { { "testuser_1", "Test@123" }, { "testuser_1", "Test@123" }};
+  }
+  // Here we are calling the Data Provider object with its Name
+  atTest(dataProvider = "Authentication")</t>
+  </si>
+  <si>
+    <t>ISuiteListener - onStart() &amp; onFinish()</t>
+  </si>
+  <si>
+    <t>ITestListner - OnStart(),OnFInsih(),OnTestFailure(),OnTestSkipped()</t>
+  </si>
+  <si>
+    <t>public class Listener implements ITestListener, ISuiteListener, IInvokedMethodListener {
+ // This belongs to ISuiteListener and will execute before the Suite start
+ atOverride
+ public void onStart(ISuite arg0) {
+  Reporter.log("About to begin executing Suite " + arg0.getName(), true);
+ }
+ // This belongs to ISuiteListener and will execute, once the Suite is finished
+ atOverride
+ public void onFinish(ISuite arg0) {
+  Reporter.log("About to end executing Suite " + arg0.getName(), true);</t>
+  </si>
+  <si>
+    <t>selectbyvalue,index.visibletext</t>
+  </si>
+  <si>
+    <t>elementnot visible,ElementNotSelectableException,NoSuchElementException,NoAlertPresentException</t>
+  </si>
+  <si>
+    <t>browser,platform</t>
+  </si>
+  <si>
+    <t>implicit,explicit,fluent
+explicit - 
+WebDriverWait wait = new WebDriverWait(driver, 10);
+WebElement element = wait.until(ExpectedConditions.elementToBeClickable(By.id("someid")));</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,6 +918,27 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF38393A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF38393A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF38393A"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -999,16 +1276,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1016,7 +1293,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1029,7 +1306,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1037,7 +1314,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30">
@@ -1045,25 +1322,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="60">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>54</v>
+      <c r="B8" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1071,7 +1351,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1079,7 +1359,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1087,13 +1367,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
@@ -1112,89 +1395,67 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>52</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B19" s="3"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="30">
-      <c r="A23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>59</v>
+      <c r="A21" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>103</v>
-      </c>
-      <c r="B24" s="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1222,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1234,26 +1495,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="120">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="210">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="195">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1314,153 +1575,153 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="44.25" customHeight="1">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="61.5" customHeight="1">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="36" customHeight="1">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="225">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="142.5" customHeight="1">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="135.75" customHeight="1">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="90">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1484,55 +1745,55 @@
   <sheetData>
     <row r="1" spans="1:2" ht="137.25" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="137.25" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="60">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="60">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1542,101 +1803,101 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="83.140625" customWidth="1"/>
+    <col min="3" max="3" width="89" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B1" s="4">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="4" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5">
       <c r="B3" s="4" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
       <c r="B4" s="4" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" s="4" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
       <c r="B6" s="4" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="4" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
       <c r="B8" s="4" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E8" s="5"/>
     </row>
@@ -1645,23 +1906,23 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" s="4" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="4" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45">
@@ -1669,50 +1930,162 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C17" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" s="4" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="4" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="4" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="4">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" t="s">
         <v>144</v>
       </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="4">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="4">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="4">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="4">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="4">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1751,67 +2124,182 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="57" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="95" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="39.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="105">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>67</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>157</v>
+      </c>
       <c r="B5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45">
-      <c r="A6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>71</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>160</v>
+      </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45">
+      <c r="B9" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="B15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="19.5" customHeight="1">
+      <c r="B16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="177.75" customHeight="1">
+      <c r="B17" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1"/>
+    <row r="19" spans="1:2" hidden="1"/>
+    <row r="20" spans="1:2" hidden="1">
+      <c r="A20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1">
+      <c r="B21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="285">
+      <c r="B22" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1831,35 +2319,35 @@
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30">
       <c r="B6" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1883,65 +2371,65 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30">
       <c r="A1" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" s="3" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="3" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30">
       <c r="B6" s="3" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="B7" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" s="3" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
       <c r="B11" s="3" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" s="3" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
few extra things added, jenkins also done
</commit_message>
<xml_diff>
--- a/SelJavaAppium.xlsx
+++ b/SelJavaAppium.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="678" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="678" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Selenium" sheetId="1" r:id="rId1"/>
     <sheet name="Java" sheetId="2" r:id="rId2"/>
     <sheet name="Appium" sheetId="3" r:id="rId3"/>
     <sheet name="Framework design" sheetId="4" r:id="rId4"/>
-    <sheet name="SQL" sheetId="5" r:id="rId5"/>
+    <sheet name="Jenkins" sheetId="5" r:id="rId5"/>
     <sheet name="Manual Testing" sheetId="6" r:id="rId6"/>
     <sheet name="TestNG" sheetId="7" r:id="rId7"/>
     <sheet name="Maven" sheetId="8" r:id="rId8"/>
     <sheet name="GIT" sheetId="9" r:id="rId9"/>
-    <sheet name="Jenkins" sheetId="10" r:id="rId10"/>
+    <sheet name="SQL" sheetId="10" r:id="rId10"/>
     <sheet name="Mobile app testing" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="220">
   <si>
     <t>Difference between RC and Webdriver</t>
   </si>
@@ -406,11 +406,6 @@
     <t>Limitations of using Appium</t>
   </si>
   <si>
-    <t>Appium does not support testing of Android Version lower than 4.2
-Limited support for hybrid app testing. E.g., not possible to test the switching action of application from the web app to native and vice-versa
-No support to run Appium Inspector on Microsoft Windows</t>
-  </si>
-  <si>
     <t>UIAutomateviewer</t>
   </si>
   <si>
@@ -891,6 +886,128 @@
 explicit - 
 WebDriverWait wait = new WebDriverWait(driver, 10);
 WebElement element = wait.until(ExpectedConditions.elementToBeClickable(By.id("someid")));</t>
+  </si>
+  <si>
+    <t>Simulator and emulator</t>
+  </si>
+  <si>
+    <t>Simulator: It is an electronic network simulation equipment or a base station equipment for CDMA/CMA mobile phones. It helps in latching home networks without roaming services and can make Voice; Data calls, SMS,
+Emulator: It is a software to test mobile application without a live handset</t>
+  </si>
+  <si>
+    <t>A/B testing</t>
+  </si>
+  <si>
+    <t>A/B testing for ios includes three steps
+Configure a test: It prepares two versions of your iOS app (A&amp;B) and test metric
+Test: Tests two iOS versions above on devices simultaneously
+Analyze: It select and measure better version to release</t>
+  </si>
+  <si>
+    <t>Unique tests for mobile apps</t>
+  </si>
+  <si>
+    <t>1.Installation
+2.Application launching without having network
+3.Uninstallation of app
+4.Orientation of app if it supports
+5.Testing application performance on a different kind of devices and network scenarios
+6.Testing the application response how it is responding</t>
+  </si>
+  <si>
+    <t>Performance testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load testing </t>
+  </si>
+  <si>
+    <t>Stress testing</t>
+  </si>
+  <si>
+    <t>Load testing is meant to test the system by constantly and steadily increasing the load on the system till the time it reaches the threshold limit. Eg."N" no of Drivers starting the trip at same time</t>
+  </si>
+  <si>
+    <t>Testing the application for performance, Eg different n/w requirements,battery peorfirmance</t>
+  </si>
+  <si>
+    <t>max 500 cars added into the system and checking how it responds</t>
+  </si>
+  <si>
+    <t>Appium does not support testing of Android Version lower than 4.2
+Limited support for hybrid app testing. E.g., not possible to test the switching action of application from the web app to native and vice-versa
+No support for toast messages
+No support to run Appium Inspector on Microsoft Windows</t>
+  </si>
+  <si>
+    <t>Advantages</t>
+  </si>
+  <si>
+    <t>multi language support
+supports IOS,android
+supports native,web,hybrid apps</t>
+  </si>
+  <si>
+    <t>Installations</t>
+  </si>
+  <si>
+    <t>What is Jenkins?</t>
+  </si>
+  <si>
+    <t>It’s a continous integration tool, where it builds,tests the code wheneever the dev checks in his code to the repository. It reveals integration issues
+User --&gt;local --&gt;central --&gt; CI--&gt; results</t>
+  </si>
+  <si>
+    <t>1. download war file from web</t>
+  </si>
+  <si>
+    <t>2. Install jenkins for windows</t>
+  </si>
+  <si>
+    <t>3. Type localhost:8080</t>
+  </si>
+  <si>
+    <t>4. In "Manage Jenkins" set up all the path like JDK,GIT path etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Create "new free style project" </t>
+  </si>
+  <si>
+    <t>6. Give GIT https path</t>
+  </si>
+  <si>
+    <t>7. Check Poll SCM - if there is any source code changes then only build triggers</t>
+  </si>
+  <si>
+    <t>8. Write * * * * * for jenkins to build and run everytime when there is code checkin</t>
+  </si>
+  <si>
+    <t>9. Click on save and apply</t>
+  </si>
+  <si>
+    <t>10. Check codes into Git - Jenkins start building the project and tests the regression test case</t>
+  </si>
+  <si>
+    <t>11. In o/p console it shows the results</t>
+  </si>
+  <si>
+    <t>12 In project--&gt; dashboard ---&gt;shows weather report if build is success or failure(bright sunny for success,cloudy for failure)</t>
+  </si>
+  <si>
+    <t>1)java setup 1.7+
+2).net framework
+3)mobile settings - developer options
+4)adk bundle download from android
+5)setup environment variables - raman and type as "adb devices" in cmd prompt
+6)appium server download(it has node.js in it)
+7)ADT plugin setup in eclipse and download all required info
+8)Maven set up and adding dependencies for created maven project
+dependencies - junit,testng,selenium,appium,gson
+or create normal project and add jars as mentioned below
+9)appium jar
+10)webdriver jar
+11)gson jar
+12)APK install in folder and set the path
+13)C:\Users\admin\android-sdks\tools - UIautomater</t>
   </si>
 </sst>
 </file>
@@ -1279,7 +1396,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1301,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="90">
+    <row r="3" spans="1:2" ht="75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1330,7 +1447,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1343,7 +1460,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1375,7 +1492,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1406,7 +1523,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30">
@@ -1419,7 +1536,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="3"/>
     </row>
@@ -1471,7 +1588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -1483,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1495,45 +1614,75 @@
   <sheetData>
     <row r="1" spans="1:2" ht="120">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="195">
       <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="B8" s="3"/>
+    </row>
+    <row r="4" spans="1:2" ht="84.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="90">
+      <c r="A5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="105">
+      <c r="A6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30">
+      <c r="A7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45">
+      <c r="A8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="B9" s="3"/>
+      <c r="A9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" s="3"/>
@@ -1731,10 +1880,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1753,31 +1902,31 @@
     </row>
     <row r="2" spans="1:2" ht="137.25" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="68.25" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="75">
+      <c r="A4" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="60">
-      <c r="A5" t="s">
-        <v>85</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>110</v>
@@ -1785,15 +1934,31 @@
     </row>
     <row r="6" spans="1:2" ht="60">
       <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="60">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>90</v>
+    </row>
+    <row r="8" spans="1:2" ht="225">
+      <c r="A8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1820,84 +1985,84 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" s="4">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5">
       <c r="B3" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
       <c r="B4" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
       <c r="B6" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
       <c r="B8" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E8" s="5"/>
     </row>
@@ -1906,23 +2071,23 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" t="s">
         <v>127</v>
-      </c>
-      <c r="C13" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45">
@@ -1930,50 +2095,50 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -1981,39 +2146,39 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="B26" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="2:3">
@@ -2021,39 +2186,39 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="2:3">
       <c r="B32" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="2:3">
@@ -2061,7 +2226,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="2:3">
@@ -2069,7 +2234,7 @@
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="2:3">
@@ -2077,7 +2242,7 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="2:3">
@@ -2085,7 +2250,7 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2098,12 +2263,90 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="49.28515625" customWidth="1"/>
+    <col min="2" max="2" width="85.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="45">
+      <c r="A1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30">
+      <c r="B13" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2126,8 +2369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2144,7 +2387,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="105">
+    <row r="2" spans="1:2" ht="90">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
@@ -2154,147 +2397,147 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
         <v>154</v>
-      </c>
-      <c r="B3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
         <v>157</v>
-      </c>
-      <c r="B5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45">
       <c r="B9" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="B15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1">
       <c r="B16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="177.75" customHeight="1">
       <c r="B17" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:2" hidden="1"/>
     <row r="19" spans="1:2" hidden="1"/>
     <row r="20" spans="1:2" hidden="1">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:2" hidden="1">
       <c r="B21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="285">
       <c r="B22" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" t="s">
         <v>163</v>
-      </c>
-      <c r="B27" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="B28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="B29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="B30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="B31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="B32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2371,65 +2614,65 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30">
       <c r="A1" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30">
       <c r="B6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="B7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
       <c r="B11" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progs of java and selenium to be read and written
</commit_message>
<xml_diff>
--- a/SelJavaAppium.xlsx
+++ b/SelJavaAppium.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="678" firstSheet="5" activeTab="14"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="828" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Selenium" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,16 @@
     <sheet name="SQL" sheetId="10" r:id="rId10"/>
     <sheet name="Mobile app testing" sheetId="11" r:id="rId11"/>
     <sheet name="Agile Process" sheetId="12" r:id="rId12"/>
-    <sheet name="basic linux" sheetId="13" r:id="rId13"/>
-    <sheet name="Sel Pro" sheetId="14" r:id="rId14"/>
-    <sheet name="Java progs" sheetId="15" r:id="rId15"/>
+    <sheet name="Sel Progs" sheetId="14" r:id="rId13"/>
+    <sheet name="Java progs" sheetId="15" r:id="rId14"/>
+    <sheet name="basic linux" sheetId="13" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="372">
   <si>
     <t>Difference between RC and Webdriver</t>
   </si>
@@ -1534,6 +1534,153 @@
   System.out.println("Max is " + max);
  }
 }</t>
+  </si>
+  <si>
+    <t>leap year or not</t>
+  </si>
+  <si>
+    <t>pyramid of stars</t>
+  </si>
+  <si>
+    <t>swap 2 numbers</t>
+  </si>
+  <si>
+    <t>triangle shape</t>
+  </si>
+  <si>
+    <t>diamond shape</t>
+  </si>
+  <si>
+    <t>union of arrays</t>
+  </si>
+  <si>
+    <t>intersection of arrays</t>
+  </si>
+  <si>
+    <t>String buffer methods</t>
+  </si>
+  <si>
+    <t>String methods</t>
+  </si>
+  <si>
+    <t>String reverse</t>
+  </si>
+  <si>
+    <t>floyds triangle</t>
+  </si>
+  <si>
+    <t>compare string</t>
+  </si>
+  <si>
+    <t>substring of a string</t>
+  </si>
+  <si>
+    <t>get url</t>
+  </si>
+  <si>
+    <t>get title</t>
+  </si>
+  <si>
+    <t>get current url</t>
+  </si>
+  <si>
+    <t>get text</t>
+  </si>
+  <si>
+    <t>refresh</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>findelement</t>
+  </si>
+  <si>
+    <t>findelements</t>
+  </si>
+  <si>
+    <t>all webelements</t>
+  </si>
+  <si>
+    <t>get window handle</t>
+  </si>
+  <si>
+    <t>get window handles</t>
+  </si>
+  <si>
+    <t>switchtowindow</t>
+  </si>
+  <si>
+    <t>implicit wait</t>
+  </si>
+  <si>
+    <t>expected conditions</t>
+  </si>
+  <si>
+    <t>draggable</t>
+  </si>
+  <si>
+    <t>droppable</t>
+  </si>
+  <si>
+    <t>resizeable</t>
+  </si>
+  <si>
+    <t>selectable</t>
+  </si>
+  <si>
+    <t>sortable</t>
+  </si>
+  <si>
+    <t>autocomplete</t>
+  </si>
+  <si>
+    <t>accordian</t>
+  </si>
+  <si>
+    <t>datepicker</t>
+  </si>
+  <si>
+    <t>slider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menu </t>
+  </si>
+  <si>
+    <t>tabs</t>
+  </si>
+  <si>
+    <t>tooltip</t>
+  </si>
+  <si>
+    <t>windows</t>
+  </si>
+  <si>
+    <t>submit button clicked</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>3 types</t>
+  </si>
+  <si>
+    <t>alert box</t>
+  </si>
+  <si>
+    <t>reading a table and fetching value from it</t>
+  </si>
+  <si>
+    <t>Actions class</t>
+  </si>
+  <si>
+    <t>iframes</t>
   </si>
 </sst>
 </file>
@@ -1615,7 +1762,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
@@ -1637,6 +1784,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1934,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2554,6 +2702,374 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="48.85546875" customWidth="1"/>
+    <col min="2" max="2" width="100.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="206.25" customHeight="1">
+      <c r="A1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>344</v>
+      </c>
+      <c r="B10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>366</v>
+      </c>
+      <c r="B32" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>370</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="99.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="266.25" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="243.75" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="303.75" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="279" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="318.75" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="266.25" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="358.5" customHeight="1">
+      <c r="A7" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="291" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="304.5" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="376.5" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="59.25" customHeight="1">
+      <c r="A11" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="7" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="7" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="7" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="7" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="7" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2574,132 +3090,6 @@
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="100.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="364.5" customHeight="1">
-      <c r="A1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="31.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="99.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="266.25" customHeight="1">
-      <c r="A1" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="243.75" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="303.75" customHeight="1">
-      <c r="A3" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="279" customHeight="1">
-      <c r="A4" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="318.75" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="266.25" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="358.5" customHeight="1">
-      <c r="A7" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="291" customHeight="1">
-      <c r="A8" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="304.5" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="376.5" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="373.5" customHeight="1"/>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>